<commit_message>
Proxy update; move prototypeJS to dependency; update doc;
</commit_message>
<xml_diff>
--- a/doc/Design.xlsx
+++ b/doc/Design.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="26835" windowHeight="14880"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="26835" windowHeight="14880" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Proxy" sheetId="1" r:id="rId1"/>
@@ -1029,7 +1029,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10:E10"/>
     </sheetView>
   </sheetViews>
@@ -1443,8 +1443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:J10"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1556,6 +1556,11 @@
         <v>44</v>
       </c>
     </row>
+    <row r="8" spans="2:10">
+      <c r="F8" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
     <row r="9" spans="2:10">
       <c r="B9" s="22" t="s">
         <v>50</v>
@@ -1569,8 +1574,8 @@
       <c r="E9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="23" t="s">
-        <v>33</v>
+      <c r="F9" s="22" t="s">
+        <v>45</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>49</v>
@@ -1585,9 +1590,6 @@
       </c>
       <c r="C10" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="F10" s="22" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reactive pattern update; view.preview; item provider
</commit_message>
<xml_diff>
--- a/doc/Design.xlsx
+++ b/doc/Design.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="26835" windowHeight="14880"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="26835" windowHeight="14880" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Proxy" sheetId="1" r:id="rId1"/>
     <sheet name="Action" sheetId="2" r:id="rId2"/>
     <sheet name="Naming" sheetId="3" r:id="rId3"/>
+    <sheet name="Test" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="135">
   <si>
     <t>Client</t>
   </si>
@@ -510,6 +511,47 @@
   </si>
   <si>
     <t>get('view.grid')</t>
+  </si>
+  <si>
+    <t>Store modified items</t>
+  </si>
+  <si>
+    <t>App.array</t>
+  </si>
+  <si>
+    <t>Item.property</t>
+  </si>
+  <si>
+    <t>undo</t>
+  </si>
+  <si>
+    <t>edit</t>
+  </si>
+  <si>
+    <t>Save</t>
+  </si>
+  <si>
+    <t>Update</t>
+  </si>
+  <si>
+    <t>push(this)</t>
+  </si>
+  <si>
+    <t>this.modified = true</t>
+  </si>
+  <si>
+    <t>this.modified = false</t>
+  </si>
+  <si>
+    <t>array.indexOf(this)
+delete
+compact</t>
+  </si>
+  <si>
+    <t>array.each(item.put)</t>
+  </si>
+  <si>
+    <t>this.items.filter.each(item.put)</t>
   </si>
 </sst>
 </file>
@@ -717,7 +759,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -836,6 +878,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1137,7 +1182,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -1775,7 +1820,7 @@
   <dimension ref="C2:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1836,4 +1881,83 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="3" width="21.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4">
+      <c r="A2" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="B4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45">
+      <c r="A5" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="34" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>